<commit_message>
New top 10 template
</commit_message>
<xml_diff>
--- a/resource/TEMPLATE_top_10_stocks.xlsx
+++ b/resource/TEMPLATE_top_10_stocks.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15902\go\src\github.com\skeyic\ark-robot\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\COCOA\Hole\ARK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D2624D-C515-4D91-A9B7-39EF721B64E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC1A62A-20C1-4662-9334-D3CA49B120C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="30" windowWidth="28035" windowHeight="20475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARKG" sheetId="6" r:id="rId1"/>
-    <sheet name="ARKK" sheetId="5" r:id="rId2"/>
-    <sheet name="ARKQ" sheetId="4" r:id="rId3"/>
-    <sheet name="ARKW" sheetId="3" r:id="rId4"/>
-    <sheet name="ARKF" sheetId="2" r:id="rId5"/>
+    <sheet name="ARKK" sheetId="12" r:id="rId2"/>
+    <sheet name="ARKQ" sheetId="11" r:id="rId3"/>
+    <sheet name="ARKW" sheetId="10" r:id="rId4"/>
+    <sheet name="ARKF" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="26">
   <si>
     <t>股票代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,66 +41,6 @@
   <si>
     <t>持有市值</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQ</t>
-  </si>
-  <si>
-    <t>SQUARE INC - A</t>
-  </si>
-  <si>
-    <t>PYPL</t>
-  </si>
-  <si>
-    <t>PAYPAL HOLDINGS INC</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>ZILLOW GROUP INC - C</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>SILVERGATE CAPITAL CORP-CL A</t>
-  </si>
-  <si>
-    <t>ICE</t>
-  </si>
-  <si>
-    <t>INTERCONTINENTAL EXCHANGE IN</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>SEA LTD-ADR</t>
-  </si>
-  <si>
-    <t>TCEHY</t>
-  </si>
-  <si>
-    <t>TENCENT HOLDINGS LTD-UNS ADR</t>
-  </si>
-  <si>
-    <t>PINS</t>
-  </si>
-  <si>
-    <t>PINTEREST INC- CLASS A</t>
-  </si>
-  <si>
-    <t>SHOP</t>
-  </si>
-  <si>
-    <t>SHOPIFY INC - CLASS A</t>
-  </si>
-  <si>
-    <t>ADYEN</t>
-  </si>
-  <si>
-    <t>ADYEN NV</t>
   </si>
   <si>
     <t>TDOC</t>
@@ -163,108 +103,6 @@
     <t>FATE THERAPEUTICS INC</t>
   </si>
   <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>TESLA INC</t>
-  </si>
-  <si>
-    <t>ROKU</t>
-  </si>
-  <si>
-    <t>ROKU INC</t>
-  </si>
-  <si>
-    <t>BIDU</t>
-  </si>
-  <si>
-    <t>BAIDU INC - SPON ADR</t>
-  </si>
-  <si>
-    <t>SPOT</t>
-  </si>
-  <si>
-    <t>SPOTIFY TECHNOLOGY SA</t>
-  </si>
-  <si>
-    <t>CRSP</t>
-  </si>
-  <si>
-    <t>CRISPR THERAPEUTICS AG</t>
-  </si>
-  <si>
-    <t>ZM</t>
-  </si>
-  <si>
-    <t>ZOOM VIDEO COMMUNICATIONS-A</t>
-  </si>
-  <si>
-    <t>TRMB</t>
-  </si>
-  <si>
-    <t>TRIMBLE INC</t>
-  </si>
-  <si>
-    <t>JD</t>
-  </si>
-  <si>
-    <t>JD.COM INC-ADR</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>DEERE &amp; CO</t>
-  </si>
-  <si>
-    <t>KTOS</t>
-  </si>
-  <si>
-    <t>KRATOS DEFENSE &amp; SECURITY</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
-    <t>ALPHABET INC-CL C</t>
-  </si>
-  <si>
-    <t>TER</t>
-  </si>
-  <si>
-    <t>TERADYNE INC</t>
-  </si>
-  <si>
-    <t>NXPI</t>
-  </si>
-  <si>
-    <t>NXP SEMICONDUCTORS NV</t>
-  </si>
-  <si>
-    <t>KMTUY</t>
-  </si>
-  <si>
-    <t>KOMATSU LTD -SPONS ADR</t>
-  </si>
-  <si>
-    <t>GBTC</t>
-  </si>
-  <si>
-    <t>GRAYSCALE BITCOIN TRUST BTC</t>
-  </si>
-  <si>
-    <t>TWTR</t>
-  </si>
-  <si>
-    <t>TWITTER INC</t>
-  </si>
-  <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>OPENDOOR TECHNOLOGIES INC</t>
-  </si>
-  <si>
     <t>本次持仓</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -281,9 +119,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -394,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,9 +249,10 @@
     <xf numFmtId="10" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1047,22 +885,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>ARKK</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>前</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>10</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>持仓</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1138,7 +975,17 @@
       </c:spPr>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5162382225157637E-2"/>
+          <c:y val="0.12734458459711981"/>
+          <c:w val="0.93561524992862133"/>
+          <c:h val="0.82194882802825553"/>
+        </c:manualLayout>
+      </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1148,11 +995,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKK!$C$34</c:f>
+              <c:f>ARKK!$D$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>上次持仓</c:v>
+                  <c:v>本次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1188,80 +1035,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQ</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TDOC</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ROKU</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Z</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BIDU</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>SPOT</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>CRSP</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SHOP</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ZM</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKK!$C$35:$C$44</c:f>
+              <c:f>ARKK!$D$35:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1071</c:v>
+                  <c:v>7.1800000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4899999999999999E-2</c:v>
+                  <c:v>5.04E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8400000000000001E-2</c:v>
+                  <c:v>4.8500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6099999999999997E-2</c:v>
+                  <c:v>4.5400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5099999999999999E-2</c:v>
+                  <c:v>4.4600000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3799999999999997E-2</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1199999999999999E-2</c:v>
+                  <c:v>3.9199999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0200000000000001E-2</c:v>
+                  <c:v>3.6900000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0200000000000001E-2</c:v>
+                  <c:v>3.6499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-968B-4DAE-8450-416463F91C31}"/>
+              <c16:uniqueId val="{00000000-79D1-4572-A10F-11B24A6DCA13}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1270,11 +1117,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKK!$D$34</c:f>
+              <c:f>ARKK!$C$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>本次持仓</c:v>
+                  <c:v>上次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1310,80 +1157,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQ</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TDOC</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ROKU</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Z</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BIDU</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>SPOT</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>CRSP</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SHOP</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ZM</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKK!$D$35:$D$44</c:f>
+              <c:f>ARKK!$C$35:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.10680000000000001</c:v>
+                  <c:v>7.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4100000000000004E-2</c:v>
+                  <c:v>5.2400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.67E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6000000000000001E-2</c:v>
+                  <c:v>4.4400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6200000000000003E-2</c:v>
+                  <c:v>4.5499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.44E-2</c:v>
+                  <c:v>3.9399999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1699999999999999E-2</c:v>
+                  <c:v>3.8699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0700000000000002E-2</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9899999999999999E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9399999999999999E-2</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-968B-4DAE-8450-416463F91C31}"/>
+              <c16:uniqueId val="{00000001-79D1-4572-A10F-11B24A6DCA13}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1398,12 +1245,12 @@
         <c:gapWidth val="160"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="1122623519"/>
-        <c:axId val="1122631839"/>
+        <c:axId val="1294345615"/>
+        <c:axId val="1294351023"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1122623519"/>
+        <c:axId val="1294345615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1287,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1122631839"/>
+        <c:crossAx val="1294351023"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1448,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1122631839"/>
+        <c:axId val="1294351023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1314,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1479,7 +1326,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1498,7 +1345,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1122623519"/>
+        <c:crossAx val="1294345615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1619,22 +1466,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>ARKQ</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>前</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>10</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>持仓</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1710,7 +1556,17 @@
       </c:spPr>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5162382225157637E-2"/>
+          <c:y val="0.12734458459711981"/>
+          <c:w val="0.93561524992862133"/>
+          <c:h val="0.82194882802825553"/>
+        </c:manualLayout>
+      </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1720,11 +1576,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKQ!$C$34</c:f>
+              <c:f>ARKQ!$D$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>上次持仓</c:v>
+                  <c:v>本次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1760,80 +1616,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BIDU</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TRMB</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>JD</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DE</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>KTOS</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>GOOG</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>TER</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>NXPI</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>KMTUY</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKQ!$C$35:$C$44</c:f>
+              <c:f>ARKQ!$D$35:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1079</c:v>
+                  <c:v>7.1800000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4199999999999998E-2</c:v>
+                  <c:v>5.04E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.21E-2</c:v>
+                  <c:v>4.8500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6899999999999997E-2</c:v>
+                  <c:v>4.5400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6100000000000002E-2</c:v>
+                  <c:v>4.4600000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9699999999999999E-2</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8199999999999998E-2</c:v>
+                  <c:v>3.9199999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7499999999999999E-2</c:v>
+                  <c:v>3.6900000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.39E-2</c:v>
+                  <c:v>3.6499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.32E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-32C8-44C6-9E00-21B8F986A755}"/>
+              <c16:uniqueId val="{00000000-4317-44FD-9A90-1E3E2EB2B5B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1842,11 +1698,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKQ!$D$34</c:f>
+              <c:f>ARKQ!$C$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>本次持仓</c:v>
+                  <c:v>上次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1882,80 +1738,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BIDU</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>TRMB</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>JD</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DE</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>KTOS</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>GOOG</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>TER</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>NXPI</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>KMTUY</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKQ!$D$35:$D$44</c:f>
+              <c:f>ARKQ!$C$35:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1077</c:v>
+                  <c:v>7.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5300000000000002E-2</c:v>
+                  <c:v>5.2400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1799999999999999E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9799999999999997E-2</c:v>
+                  <c:v>4.4400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5400000000000003E-2</c:v>
+                  <c:v>4.5499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.04</c:v>
+                  <c:v>3.9399999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8800000000000001E-2</c:v>
+                  <c:v>3.8699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7400000000000003E-2</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4500000000000003E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2800000000000003E-2</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-32C8-44C6-9E00-21B8F986A755}"/>
+              <c16:uniqueId val="{00000001-4317-44FD-9A90-1E3E2EB2B5B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1970,12 +1826,12 @@
         <c:gapWidth val="160"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="1122628927"/>
-        <c:axId val="1122629343"/>
+        <c:axId val="1294345615"/>
+        <c:axId val="1294351023"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1122628927"/>
+        <c:axId val="1294345615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1853,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2012,7 +1868,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1122629343"/>
+        <c:crossAx val="1294351023"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,7 +1876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1122629343"/>
+        <c:axId val="1294351023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2039,7 +1895,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2051,11 +1907,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2070,7 +1926,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1122628927"/>
+        <c:crossAx val="1294345615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2191,22 +2047,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>ARKW</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>前</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>10</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>持仓</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2282,7 +2137,17 @@
       </c:spPr>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5162382225157637E-2"/>
+          <c:y val="0.12734458459711981"/>
+          <c:w val="0.93561524992862133"/>
+          <c:h val="0.82194882802825553"/>
+        </c:manualLayout>
+      </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2292,11 +2157,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKW!$C$34</c:f>
+              <c:f>ARKW!$D$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>上次持仓</c:v>
+                  <c:v>本次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2332,80 +2197,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQ</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>GBTC</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TDOC</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ROKU</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>SPOT</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>SHOP</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>TWTR</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>OPEN</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ZM</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKW!$C$35:$C$44</c:f>
+              <c:f>ARKW!$D$35:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.10680000000000001</c:v>
+                  <c:v>7.1800000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5E-2</c:v>
+                  <c:v>5.04E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3999999999999999E-2</c:v>
+                  <c:v>4.8500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0500000000000001E-2</c:v>
+                  <c:v>4.5400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9E-2</c:v>
+                  <c:v>4.4600000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4599999999999999E-2</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4200000000000001E-2</c:v>
+                  <c:v>3.9199999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.81E-2</c:v>
+                  <c:v>3.6900000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.29E-2</c:v>
+                  <c:v>3.6499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2499999999999999E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E8D-47D1-92B6-27FDCFD03D8A}"/>
+              <c16:uniqueId val="{00000000-8B07-45BE-9F4B-FAD47E519DF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2414,11 +2279,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKW!$D$34</c:f>
+              <c:f>ARKW!$C$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>本次持仓</c:v>
+                  <c:v>上次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2454,80 +2319,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>TSLA</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SQ</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>GBTC</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TDOC</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ROKU</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>SPOT</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>SHOP</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>TWTR</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>OPEN</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ZM</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKW!$D$35:$D$44</c:f>
+              <c:f>ARKW!$C$35:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1061</c:v>
+                  <c:v>7.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4100000000000002E-2</c:v>
+                  <c:v>5.2400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.57E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0099999999999997E-2</c:v>
+                  <c:v>4.4400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8800000000000001E-2</c:v>
+                  <c:v>4.5499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.49E-2</c:v>
+                  <c:v>3.9399999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3799999999999997E-2</c:v>
+                  <c:v>3.8699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7799999999999998E-2</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2800000000000001E-2</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1E8D-47D1-92B6-27FDCFD03D8A}"/>
+              <c16:uniqueId val="{00000001-8B07-45BE-9F4B-FAD47E519DF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2542,12 +2407,12 @@
         <c:gapWidth val="160"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="1294746415"/>
-        <c:axId val="1294746831"/>
+        <c:axId val="1294345615"/>
+        <c:axId val="1294351023"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1294746415"/>
+        <c:axId val="1294345615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2569,7 +2434,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2584,7 +2449,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1294746831"/>
+        <c:crossAx val="1294351023"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2592,7 +2457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1294746831"/>
+        <c:axId val="1294351023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2476,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2623,11 +2488,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2642,7 +2507,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1294746415"/>
+        <c:crossAx val="1294345615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,22 +2628,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>ARKF</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>前</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US"/>
               <a:t>10</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:rPr lang="zh-CN"/>
               <a:t>持仓</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2854,7 +2718,17 @@
       </c:spPr>
     </c:backWall>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5162382225157637E-2"/>
+          <c:y val="0.12734458459711981"/>
+          <c:w val="0.93561524992862133"/>
+          <c:h val="0.82194882802825553"/>
+        </c:manualLayout>
+      </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2864,11 +2738,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKF!$C$34</c:f>
+              <c:f>ARKF!$D$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>上次持仓</c:v>
+                  <c:v>本次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2904,80 +2778,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>SQ</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PYPL</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Z</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SI</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ICE</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>SE</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>TCEHY</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>PINS</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SHOP</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ADYEN</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKF!$C$35:$C$44</c:f>
+              <c:f>ARKF!$D$35:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.1047</c:v>
+                  <c:v>7.1800000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3800000000000001E-2</c:v>
+                  <c:v>5.04E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9000000000000002E-2</c:v>
+                  <c:v>4.8500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2999999999999997E-2</c:v>
+                  <c:v>4.5400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>4.4600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3.9199999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3.6900000000000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5099999999999999E-2</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.44E-2</c:v>
+                  <c:v>3.6499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1099999999999999E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-314C-4760-8686-608ED5E46459}"/>
+              <c16:uniqueId val="{00000000-2240-48D3-81A4-D1025E404CBE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2986,11 +2860,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ARKF!$D$34</c:f>
+              <c:f>ARKF!$C$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>本次持仓</c:v>
+                  <c:v>上次持仓</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3026,80 +2900,80 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>SQ</c:v>
+                  <c:v>TDOC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PYPL</c:v>
+                  <c:v>PACB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Z</c:v>
+                  <c:v>EXAS</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SI</c:v>
+                  <c:v>REGN</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ICE</c:v>
+                  <c:v>TWST</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>SE</c:v>
+                  <c:v>VRTX</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>TCEHY</c:v>
+                  <c:v>NVS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>PINS</c:v>
+                  <c:v>TAK UN</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>SHOP</c:v>
+                  <c:v>RHHBY</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>ADYEN</c:v>
+                  <c:v>FATE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ARKF!$D$35:$D$44</c:f>
+              <c:f>ARKF!$C$35:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.104</c:v>
+                  <c:v>7.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4199999999999998E-2</c:v>
+                  <c:v>5.2400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0900000000000001E-2</c:v>
+                  <c:v>4.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2999999999999997E-2</c:v>
+                  <c:v>4.4400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9E-2</c:v>
+                  <c:v>4.5499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>3.9399999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.8699999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>3.6400000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4299999999999997E-2</c:v>
+                  <c:v>3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1800000000000002E-2</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-314C-4760-8686-608ED5E46459}"/>
+              <c16:uniqueId val="{00000001-2240-48D3-81A4-D1025E404CBE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3114,12 +2988,12 @@
         <c:gapWidth val="160"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="1294767215"/>
-        <c:axId val="1294769711"/>
+        <c:axId val="1294345615"/>
+        <c:axId val="1294351023"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1294767215"/>
+        <c:axId val="1294345615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3141,7 +3015,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3156,7 +3030,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1294769711"/>
+        <c:crossAx val="1294351023"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3164,7 +3038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1294769711"/>
+        <c:axId val="1294351023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3183,7 +3057,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3195,11 +3069,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3214,7 +3088,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1294767215"/>
+        <c:crossAx val="1294345615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6117,26 +5991,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B720F7E0-DB44-4450-8261-0180EDEC6197}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F80DD8-E858-4CC5-AD0D-3EEB3F21F6E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6158,26 +6034,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E746E4E4-9F24-4B18-8BC1-DD67960C741A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6EEF71A-06C6-4280-9B68-B88E8931C350}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6199,26 +6077,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB31BC0-4CDB-4CCA-9983-62D4144FE51D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB47EA1B-0EBA-420E-8F20-0F8A91CC7AFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6240,26 +6120,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3002E64-9EFE-492A-BB90-1BB13686A02E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EF77032-94D5-4A8E-AC9F-60554F2E8537}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6541,15 +6423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5D3B50-71B3-46D7-BAA6-A2F85D4251AD}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
   </cols>
@@ -6561,14 +6443,14 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>77</v>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -6576,10 +6458,10 @@
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C35" s="6">
         <v>7.0699999999999999E-2</v>
@@ -6587,7 +6469,7 @@
       <c r="D35" s="6">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="5">
         <v>197.95000001404699</v>
       </c>
       <c r="F35" s="5">
@@ -6596,10 +6478,10 @@
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6">
         <v>5.2400000000000002E-2</v>
@@ -6607,7 +6489,7 @@
       <c r="D36" s="6">
         <v>5.04E-2</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="5">
         <v>33.89000000136997</v>
       </c>
       <c r="F36" s="5">
@@ -6616,10 +6498,10 @@
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6">
         <v>4.87E-2</v>
@@ -6627,7 +6509,7 @@
       <c r="D37" s="6">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="5">
         <v>128.46000000540187</v>
       </c>
       <c r="F37" s="5">
@@ -6636,10 +6518,10 @@
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C38" s="6">
         <v>4.4400000000000002E-2</v>
@@ -6647,7 +6529,7 @@
       <c r="D38" s="6">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <v>471.45999995765686</v>
       </c>
       <c r="F38" s="5">
@@ -6656,10 +6538,10 @@
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C39" s="6">
         <v>4.5499999999999999E-2</v>
@@ -6667,7 +6549,7 @@
       <c r="D39" s="6">
         <v>4.4600000000000001E-2</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>141.4</v>
       </c>
       <c r="F39" s="5">
@@ -6676,10 +6558,10 @@
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C40" s="6">
         <v>3.9399999999999998E-2</v>
@@ -6687,7 +6569,7 @@
       <c r="D40" s="6">
         <v>0.04</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="5">
         <v>214.32999998362322</v>
       </c>
       <c r="F40" s="5">
@@ -6696,10 +6578,10 @@
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6">
         <v>3.8699999999999998E-2</v>
@@ -6707,7 +6589,7 @@
       <c r="D41" s="6">
         <v>3.9199999999999999E-2</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="5">
         <v>84.130000010924775</v>
       </c>
       <c r="F41" s="5">
@@ -6716,10 +6598,10 @@
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C42" s="6">
         <v>3.6400000000000002E-2</v>
@@ -6727,7 +6609,7 @@
       <c r="D42" s="6">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="5">
         <v>18.440000001017651</v>
       </c>
       <c r="F42" s="5">
@@ -6736,10 +6618,10 @@
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C43" s="6">
         <v>3.6299999999999999E-2</v>
@@ -6747,7 +6629,7 @@
       <c r="D43" s="6">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="5">
         <v>41.030000005730308</v>
       </c>
       <c r="F43" s="5">
@@ -6756,10 +6638,10 @@
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C44" s="6">
         <v>3.6999999999999998E-2</v>
@@ -6767,7 +6649,7 @@
       <c r="D44" s="6">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="5">
         <v>93.990000007903532</v>
       </c>
       <c r="F44" s="5">
@@ -6783,18 +6665,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5680B69-1748-4D53-BA8B-430C36CE1C7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9501A662-549E-4507-8C0B-B6E871543743}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
   </cols>
@@ -6806,14 +6688,14 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>77</v>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -6821,162 +6703,162 @@
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C35" s="6">
-        <v>0.1071</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="D35" s="6">
-        <v>0.10680000000000001</v>
-      </c>
-      <c r="E35" s="7">
-        <v>693.73000009812677</v>
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>197.95000001404699</v>
       </c>
       <c r="F35" s="5">
-        <v>2615799844</v>
+        <v>704598076.29999995</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6">
-        <v>6.4899999999999999E-2</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="D36" s="6">
-        <v>6.4100000000000004E-2</v>
-      </c>
-      <c r="E36" s="7">
-        <v>242.10999992978478</v>
+        <v>5.04E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>33.89000000136997</v>
       </c>
       <c r="F36" s="5">
-        <v>1586131853</v>
+        <v>494755094.30000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6">
-        <v>5.8400000000000001E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="D37" s="6">
-        <v>5.67E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>197.94999996533869</v>
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>128.46000000540187</v>
       </c>
       <c r="F37" s="5">
-        <v>1427745057</v>
+        <v>475612616.30000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C38" s="6">
-        <v>5.6099999999999997E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="D38" s="6">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E38" s="7">
-        <v>359.95999987394589</v>
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>471.45999995765686</v>
       </c>
       <c r="F38" s="5">
-        <v>1370687364</v>
+        <v>445371289.39999998</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C39" s="6">
-        <v>3.5099999999999999E-2</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="D39" s="6">
-        <v>3.6200000000000003E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>150.70999999648555</v>
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>141.4</v>
       </c>
       <c r="F39" s="5">
-        <v>857660769.39999998</v>
+        <v>437867299.80000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C40" s="6">
-        <v>3.3799999999999997E-2</v>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="D40" s="6">
-        <v>3.44E-2</v>
-      </c>
-      <c r="E40" s="7">
-        <v>264.25000001602092</v>
+        <v>0.04</v>
+      </c>
+      <c r="E40" s="5">
+        <v>214.32999998362322</v>
       </c>
       <c r="F40" s="5">
-        <v>824700731.79999995</v>
+        <v>392622768.10000002</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6">
-        <v>3.1199999999999999E-2</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="D41" s="6">
-        <v>3.1699999999999999E-2</v>
-      </c>
-      <c r="E41" s="7">
-        <v>279.88999999633307</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>84.130000010924775</v>
       </c>
       <c r="F41" s="5">
-        <v>763276543.5</v>
+        <v>385042398.19999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C42" s="6">
-        <v>3.0200000000000001E-2</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="D42" s="6">
-        <v>3.0700000000000002E-2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>130.60999999645944</v>
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>18.440000001017651</v>
       </c>
       <c r="F42" s="5">
-        <v>737788723.10000002</v>
+        <v>362403200.89999998</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6987,59 +6869,59 @@
         <v>20</v>
       </c>
       <c r="C43" s="6">
-        <v>3.0200000000000001E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="D43" s="6">
-        <v>2.9899999999999999E-2</v>
-      </c>
-      <c r="E43" s="7">
-        <v>1140.6300000772733</v>
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41.030000005730308</v>
       </c>
       <c r="F43" s="5">
-        <v>738050344.70000005</v>
+        <v>358008701.10000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C44" s="6">
-        <v>2.9000000000000001E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D44" s="6">
-        <v>2.9399999999999999E-2</v>
-      </c>
-      <c r="E44" s="7">
-        <v>346.39000001955441</v>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>93.990000007903532</v>
       </c>
       <c r="F44" s="5">
-        <v>708566377.89999998</v>
+        <v>356764704.30000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B4CDCD-4914-40BC-A939-3021ED3B00DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B80594-92D4-44C0-B254-7072F66C4F03}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
   </cols>
@@ -7051,14 +6933,14 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>77</v>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -7066,225 +6948,225 @@
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C35" s="6">
-        <v>0.1079</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="D35" s="6">
-        <v>0.1077</v>
-      </c>
-      <c r="E35" s="7">
-        <v>693.73000007460143</v>
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>197.95000001404699</v>
       </c>
       <c r="F35" s="5">
-        <v>371965538.89999998</v>
+        <v>704598076.29999995</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6">
-        <v>5.4199999999999998E-2</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="D36" s="6">
-        <v>5.5300000000000002E-2</v>
-      </c>
-      <c r="E36" s="7">
-        <v>264.25</v>
+        <v>5.04E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>33.89000000136997</v>
       </c>
       <c r="F36" s="5">
-        <v>186731734</v>
+        <v>494755094.30000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6">
-        <v>5.21E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="D37" s="6">
-        <v>5.1799999999999999E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>73.869999995885493</v>
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>128.46000000540187</v>
       </c>
       <c r="F37" s="5">
-        <v>179535347</v>
+        <v>475612616.30000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="C38" s="6">
-        <v>4.6899999999999997E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="D38" s="6">
-        <v>4.9799999999999997E-2</v>
-      </c>
-      <c r="E38" s="7">
-        <v>84.020000010384791</v>
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>471.45999995765686</v>
       </c>
       <c r="F38" s="5">
-        <v>161813613.90000001</v>
+        <v>445371289.39999998</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C39" s="6">
-        <v>4.6100000000000002E-2</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="D39" s="6">
-        <v>4.5400000000000003E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>369.48999993024017</v>
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>141.4</v>
       </c>
       <c r="F39" s="5">
-        <v>158898066</v>
+        <v>437867299.80000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C40" s="6">
-        <v>3.9699999999999999E-2</v>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="D40" s="6">
         <v>0.04</v>
       </c>
-      <c r="E40" s="7">
-        <v>26.520000007744429</v>
+      <c r="E40" s="5">
+        <v>214.32999998362322</v>
       </c>
       <c r="F40" s="5">
-        <v>136975879.59999999</v>
+        <v>392622768.10000002</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6">
-        <v>3.8199999999999998E-2</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="D41" s="6">
-        <v>3.8800000000000001E-2</v>
-      </c>
-      <c r="E41" s="7">
-        <v>2061.92</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>84.130000010924775</v>
       </c>
       <c r="F41" s="5">
-        <v>131591734.40000001</v>
+        <v>385042398.19999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C42" s="6">
-        <v>3.7499999999999999E-2</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="D42" s="6">
-        <v>3.7400000000000003E-2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>112.83000001747052</v>
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>18.440000001017651</v>
       </c>
       <c r="F42" s="5">
-        <v>129166204.40000001</v>
+        <v>362403200.89999998</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C43" s="6">
-        <v>3.39E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="D43" s="6">
-        <v>3.4500000000000003E-2</v>
-      </c>
-      <c r="E43" s="7">
-        <v>183.47000001570458</v>
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41.030000005730308</v>
       </c>
       <c r="F43" s="5">
-        <v>116825806.8</v>
+        <v>358008701.10000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="C44" s="6">
-        <v>3.32E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D44" s="6">
-        <v>3.2800000000000003E-2</v>
-      </c>
-      <c r="E44" s="7">
-        <v>31.709999997233396</v>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>93.990000007903532</v>
       </c>
       <c r="F44" s="5">
-        <v>114617095.09999999</v>
+        <v>356764704.30000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2779E1FD-482E-493C-AFDD-E630F7F9ECAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC69461-DB55-4577-ACCC-E8698B588991}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
   </cols>
@@ -7296,14 +7178,14 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>77</v>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -7311,225 +7193,225 @@
     </row>
     <row r="35" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C35" s="6">
-        <v>0.10680000000000001</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="D35" s="6">
-        <v>0.1061</v>
-      </c>
-      <c r="E35" s="7">
-        <v>693.7299999737686</v>
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>197.95000001404699</v>
       </c>
       <c r="F35" s="5">
-        <v>793398882.79999995</v>
+        <v>704598076.29999995</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6">
-        <v>5.5E-2</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="D36" s="6">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="E36" s="7">
-        <v>242.10999998221857</v>
+        <v>5.04E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>33.89000000136997</v>
       </c>
       <c r="F36" s="5">
-        <v>408476612.80000001</v>
+        <v>494755094.30000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6">
-        <v>5.3999999999999999E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="D37" s="6">
-        <v>5.57E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>50</v>
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>128.46000000540187</v>
       </c>
       <c r="F37" s="5">
-        <v>401456350</v>
+        <v>475612616.30000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C38" s="6">
-        <v>4.0500000000000001E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="D38" s="6">
-        <v>4.0099999999999997E-2</v>
-      </c>
-      <c r="E38" s="7">
-        <v>197.95</v>
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>471.45999995765686</v>
       </c>
       <c r="F38" s="5">
-        <v>301019793.69999999</v>
+        <v>445371289.39999998</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C39" s="6">
-        <v>3.9E-2</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="D39" s="6">
-        <v>3.8800000000000001E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>359.96000004967334</v>
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>141.4</v>
       </c>
       <c r="F39" s="5">
-        <v>289861749.60000002</v>
+        <v>437867299.80000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C40" s="6">
-        <v>3.4599999999999999E-2</v>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="D40" s="6">
-        <v>3.49E-2</v>
-      </c>
-      <c r="E40" s="7">
-        <v>279.88999998910879</v>
+        <v>0.04</v>
+      </c>
+      <c r="E40" s="5">
+        <v>214.32999998362322</v>
       </c>
       <c r="F40" s="5">
-        <v>256986321.40000001</v>
+        <v>392622768.10000002</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6">
-        <v>3.4200000000000001E-2</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="D41" s="6">
-        <v>3.3799999999999997E-2</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1140.6300001344573</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>84.130000010924775</v>
       </c>
       <c r="F41" s="5">
-        <v>254496225</v>
+        <v>385042398.19999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="C42" s="6">
-        <v>2.81E-2</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="D42" s="6">
-        <v>2.7799999999999998E-2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>68.099999999999994</v>
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>18.440000001017651</v>
       </c>
       <c r="F42" s="5">
-        <v>208514504.69999999</v>
+        <v>362403200.89999998</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="C43" s="6">
-        <v>2.29E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="D43" s="6">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E43" s="7">
-        <v>27.05</v>
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41.030000005730308</v>
       </c>
       <c r="F43" s="5">
-        <v>170202116.5</v>
+        <v>358008701.10000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C44" s="6">
-        <v>2.2499999999999999E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D44" s="6">
-        <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="E44" s="7">
-        <v>346.39</v>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>93.990000007903532</v>
       </c>
       <c r="F44" s="5">
-        <v>167455317.69999999</v>
+        <v>356764704.30000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6881A1E6-E610-42B7-B2DC-D2FCC1A65EF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D2EC72-2C02-44FD-AB3E-80E6A4916E2E}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.625" customWidth="1"/>
-    <col min="3" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="18.625" customWidth="1"/>
   </cols>
@@ -7541,14 +7423,14 @@
       <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>77</v>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -7562,16 +7444,16 @@
         <v>4</v>
       </c>
       <c r="C35" s="6">
-        <v>0.1047</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="D35" s="6">
-        <v>0.104</v>
-      </c>
-      <c r="E35" s="7">
-        <v>242.11000002734818</v>
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>197.95000001404699</v>
       </c>
       <c r="F35" s="5">
-        <v>442643660.30000001</v>
+        <v>704598076.29999995</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7582,16 +7464,16 @@
         <v>6</v>
       </c>
       <c r="C36" s="6">
-        <v>5.3800000000000001E-2</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="D36" s="6">
-        <v>5.4199999999999998E-2</v>
-      </c>
-      <c r="E36" s="7">
-        <v>250.35000005507186</v>
+        <v>5.04E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>33.89000000136997</v>
       </c>
       <c r="F36" s="5">
-        <v>227294016.80000001</v>
+        <v>494755094.30000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7602,16 +7484,16 @@
         <v>8</v>
       </c>
       <c r="C37" s="6">
-        <v>4.9000000000000002E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="D37" s="6">
-        <v>5.0900000000000001E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>150.71000000727381</v>
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>128.46000000540187</v>
       </c>
       <c r="F37" s="5">
-        <v>207195957.30000001</v>
+        <v>475612616.30000001</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7622,16 +7504,16 @@
         <v>10</v>
       </c>
       <c r="C38" s="6">
-        <v>4.2999999999999997E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="D38" s="6">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E38" s="7">
-        <v>138.58999996953369</v>
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>471.45999995765686</v>
       </c>
       <c r="F38" s="5">
-        <v>181958414.30000001</v>
+        <v>445371289.39999998</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7642,16 +7524,16 @@
         <v>12</v>
       </c>
       <c r="C39" s="6">
-        <v>3.9199999999999999E-2</v>
+        <v>4.5499999999999999E-2</v>
       </c>
       <c r="D39" s="6">
-        <v>3.9E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>115.31999997217821</v>
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>141.4</v>
       </c>
       <c r="F39" s="5">
-        <v>165798101</v>
+        <v>437867299.80000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7662,16 +7544,16 @@
         <v>14</v>
       </c>
       <c r="C40" s="6">
-        <v>3.6900000000000002E-2</v>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="D40" s="6">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="E40" s="7">
-        <v>234.99000001506317</v>
+        <v>0.04</v>
+      </c>
+      <c r="E40" s="5">
+        <v>214.32999998362322</v>
       </c>
       <c r="F40" s="5">
-        <v>156003046.30000001</v>
+        <v>392622768.10000002</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7682,16 +7564,16 @@
         <v>16</v>
       </c>
       <c r="C41" s="6">
-        <v>3.5999999999999997E-2</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="D41" s="6">
-        <v>3.8699999999999998E-2</v>
-      </c>
-      <c r="E41" s="7">
-        <v>82.569999994575511</v>
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>84.130000010924775</v>
       </c>
       <c r="F41" s="5">
-        <v>152217217</v>
+        <v>385042398.19999999</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7702,16 +7584,16 @@
         <v>18</v>
       </c>
       <c r="C42" s="6">
-        <v>3.5099999999999999E-2</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="D42" s="6">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>71.750000024160869</v>
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>18.440000001017651</v>
       </c>
       <c r="F42" s="5">
-        <v>148483970.30000001</v>
+        <v>362403200.89999998</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7722,16 +7604,16 @@
         <v>20</v>
       </c>
       <c r="C43" s="6">
-        <v>3.44E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="D43" s="6">
-        <v>3.4299999999999997E-2</v>
-      </c>
-      <c r="E43" s="7">
-        <v>1140.6299996863925</v>
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41.030000005730308</v>
       </c>
       <c r="F43" s="5">
-        <v>145485075.19999999</v>
+        <v>358008701.10000002</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7742,21 +7624,21 @@
         <v>22</v>
       </c>
       <c r="C44" s="6">
-        <v>3.1099999999999999E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D44" s="6">
-        <v>3.1800000000000002E-2</v>
-      </c>
-      <c r="E44" s="7">
-        <v>2314.5379305487077</v>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>93.990000007903532</v>
       </c>
       <c r="F44" s="5">
-        <v>131437980</v>
+        <v>356764704.30000001</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Support to call report with special trading percent.
</commit_message>
<xml_diff>
--- a/resource/TEMPLATE_top_10_stocks.xlsx
+++ b/resource/TEMPLATE_top_10_stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\COCOA\Hole\ARK\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31176B08-766D-4906-B8A6-B88E3331EB2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76135030-483F-4562-A7F6-986248A8578D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="135" windowWidth="21015" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7230" yWindow="540" windowWidth="22515" windowHeight="19065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ARKG" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ARKQ" sheetId="11" r:id="rId3"/>
     <sheet name="ARKW" sheetId="10" r:id="rId4"/>
     <sheet name="ARKF" sheetId="9" r:id="rId5"/>
+    <sheet name="ARKX" sheetId="13" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">ARKF!$A$1:$F$45</definedName>
@@ -25,6 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">ARKK!$A$1:$F$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">ARKQ!$A$1:$F$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">ARKW!$A$1:$F$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">ARKX!$A$1:$F$45</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>股票代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2961,6 +2963,582 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2240-48D3-81A4-D1025E404CBE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="160"/>
+        <c:gapDepth val="0"/>
+        <c:shape val="box"/>
+        <c:axId val="1294345615"/>
+        <c:axId val="1294351023"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1294345615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1294351023"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1294351023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1294345615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ARKX</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN"/>
+              <a:t>前</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>10</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN"/>
+              <a:t>持仓</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="10"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.5162382225157637E-2"/>
+          <c:y val="0.12734458459711981"/>
+          <c:w val="0.93561524992862133"/>
+          <c:h val="0.82194882802825553"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ARKX!$D$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>本次持仓</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="accent1"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ARKX!$A$35:$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>TDOC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PACB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EXAS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>REGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TWST</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VRTX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>NVS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TAK UN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RHHBY</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ARKX!$D$35:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.1800000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.04E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6299999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-132D-4036-8D54-79C6B50DEF1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ARKX!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>上次持仓</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent3"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d>
+              <a:contourClr>
+                <a:schemeClr val="accent3"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ARKX!$A$35:$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>TDOC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PACB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EXAS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>REGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TWST</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VRTX</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>NVS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>TAK UN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RHHBY</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FATE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ARKX!$C$35:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.0699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9399999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8699999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-132D-4036-8D54-79C6B50DEF1B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3342,6 +3920,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="287">
   <cs:axisTitle>
@@ -5411,6 +6026,523 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="287">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="287">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6140,6 +7272,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{789A9BE2-FD76-4459-9300-EAD1CCB0329A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6405,8 +7580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5D3B50-71B3-46D7-BAA6-A2F85D4251AD}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6650,7 +7825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9501A662-549E-4507-8C0B-B6E871543743}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
@@ -6895,7 +8070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B80594-92D4-44C0-B254-7072F66C4F03}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -7140,7 +8315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC69461-DB55-4577-ACCC-E8698B588991}">
   <dimension ref="A34:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
@@ -7624,4 +8799,249 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5386F07A-A94C-4C96-962C-6DB71FDEF6CC}">
+  <dimension ref="A34:F44"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
+    <col min="3" max="4" width="10.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="18.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="34" spans="1:6" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="6">
+        <v>7.0699999999999999E-2</v>
+      </c>
+      <c r="D35" s="6">
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>197.95000001404699</v>
+      </c>
+      <c r="F35" s="5">
+        <v>704598076.29999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="6">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="D36" s="6">
+        <v>5.04E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>33.89000000136997</v>
+      </c>
+      <c r="F36" s="5">
+        <v>494755094.30000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4.87E-2</v>
+      </c>
+      <c r="D37" s="6">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>128.46000000540187</v>
+      </c>
+      <c r="F37" s="5">
+        <v>475612616.30000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="D38" s="6">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>471.45999995765686</v>
+      </c>
+      <c r="F38" s="5">
+        <v>445371289.39999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="6">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="D39" s="6">
+        <v>4.4600000000000001E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>141.4</v>
+      </c>
+      <c r="F39" s="5">
+        <v>437867299.80000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="E40" s="5">
+        <v>214.32999998362322</v>
+      </c>
+      <c r="F40" s="5">
+        <v>392622768.10000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="6">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="D41" s="6">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>84.130000010924775</v>
+      </c>
+      <c r="F41" s="5">
+        <v>385042398.19999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="6">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="D42" s="6">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>18.440000001017651</v>
+      </c>
+      <c r="F42" s="5">
+        <v>362403200.89999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="6">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="D43" s="6">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41.030000005730308</v>
+      </c>
+      <c r="F43" s="5">
+        <v>358008701.10000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="6">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D44" s="6">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>93.990000007903532</v>
+      </c>
+      <c r="F44" s="5">
+        <v>356764704.30000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>